<commit_message>
State not mentioned → ?
</commit_message>
<xml_diff>
--- a/Project5268_P. D. Taylor(2000).xlsx
+++ b/Project5268_P. D. Taylor(2000).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remi/Desktop/Finished &amp; Uploaded copy 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjg18\GitHub\neotrans\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02360141-BE9C-CB4C-AD31-0F4E30F92CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D883FD16-2A3A-4B38-BC13-93584EAD00A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{82CB97C3-56FC-3A46-9CD0-A600CD051AFF}"/>
+    <workbookView xWindow="-15" yWindow="7080" windowWidth="15870" windowHeight="18585" xr2:uid="{82CB97C3-56FC-3A46-9CD0-A600CD051AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Project5268" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
   <si>
     <t>Charlabels</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>NT2;0=0-;1=11;2=12</t>
+  </si>
+  <si>
+    <t>N;0=0;1=1;2=?</t>
   </si>
 </sst>
 </file>
@@ -645,16 +648,16 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.33203125" customWidth="1"/>
-    <col min="2" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="83.375" customWidth="1"/>
+    <col min="2" max="3" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -676,7 +679,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -687,7 +690,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -698,7 +701,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -709,7 +712,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -720,7 +723,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -731,7 +734,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -742,7 +745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -753,7 +756,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -764,7 +767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -775,7 +778,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -786,7 +789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -797,7 +800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -808,7 +811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -819,7 +822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -830,7 +833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -841,7 +844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -852,7 +855,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -863,7 +866,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -874,18 +877,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -893,7 +896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -904,7 +907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -915,7 +918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -926,7 +929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -937,7 +940,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -948,7 +951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -959,7 +962,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -970,7 +973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -981,7 +984,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -992,7 +995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>

</xml_diff>